<commit_message>
Add hour(), minute(), second() & timevalue() functions
</commit_message>
<xml_diff>
--- a/tests/fixtures/date-time.xlsx
+++ b/tests/fixtures/date-time.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="420" windowWidth="21795" windowHeight="8985"/>
   </bookViews>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>date</t>
   </si>
@@ -98,12 +98,37 @@
   </si>
   <si>
     <t>XYZZY</t>
+  </si>
+  <si>
+    <t>Date SN</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>1:23</t>
+  </si>
+  <si>
+    <t>1.25</t>
+  </si>
+  <si>
+    <t>12:59:59 AM</t>
+  </si>
+  <si>
+    <t>1:00:00 AM</t>
+  </si>
+  <si>
+    <t>12:59:59</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -133,12 +158,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,22 +461,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C1">
         <v>0</v>
@@ -502,403 +532,748 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="C2">
+        <v>61.6</v>
+      </c>
+      <c r="D2" s="5">
+        <v>5.7638888888888885E-2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2">
+        <v>1.25</v>
+      </c>
+      <c r="H2">
+        <v>1.24</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0.67499999999999993</v>
+      </c>
+      <c r="J2">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O2" t="b">
+        <v>1</v>
+      </c>
+      <c r="P2" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q2" s="3" t="e">
+        <f>1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="3"/>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>2</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="3"/>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <f>DAY(B1)</f>
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <f t="shared" ref="C5:R5" si="0">DAY(C1)</f>
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="P5" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="Q5" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R5" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <f>DAY(B1)</f>
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:R8" si="0">DAY(C1)</f>
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P8" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q8" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R8" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:18">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:18">
       <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <f>HOUR(B2)</f>
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:R13" si="1">HOUR(C2)</f>
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P13" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R13" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <f>MINUTE(B2)</f>
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:R15" si="2">MINUTE(C2)</f>
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P15" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q15" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R15" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B16">
         <f>MONTH(B1)</f>
         <v>1</v>
       </c>
-      <c r="C13">
-        <f t="shared" ref="C13:O13" si="1">MONTH(C1)</f>
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="1"/>
+      <c r="C16">
+        <f t="shared" ref="C16:O16" si="3">MONTH(C1)</f>
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="G13">
-        <f t="shared" si="1"/>
+      <c r="G16">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="H13">
-        <f t="shared" si="1"/>
+      <c r="H16">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="I13">
-        <f t="shared" si="1"/>
+      <c r="I16">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="J13">
-        <f t="shared" si="1"/>
+      <c r="J16">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="K13">
-        <f t="shared" si="1"/>
+      <c r="K16">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="L13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="1"/>
+      <c r="L16">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="N13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="O13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="P13" t="e">
+      <c r="N16">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P16" t="e">
         <f>MONTH(P1)</f>
         <v>#NUM!</v>
       </c>
-      <c r="Q13" t="e">
+      <c r="Q16" t="e">
         <f>MONTH(Q1)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R13" t="e">
+      <c r="R16" t="e">
         <f>MONTH(R1)</f>
         <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
-      <c r="A16" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:18">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:18">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:18">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <f>SECOND(B2)</f>
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ref="C20:R20" si="4">SECOND(C2)</f>
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="7">
+        <f t="shared" si="4"/>
+        <v>54</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="4"/>
+        <v>59</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="4"/>
+        <v>59</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P20" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q20" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R20" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="21" spans="1:18">
       <c r="A21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="e">
+        <f>TIMEVALUE(B2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C22" t="e">
+        <f t="shared" ref="C22:R22" si="5">TIMEVALUE(C2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D22" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="5"/>
+        <v>5.7638888888888885E-2</v>
+      </c>
+      <c r="F22" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G22" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H22" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I22" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J22" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="5"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="5"/>
+        <v>4.1655092592592598E-2</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="5"/>
+        <v>0.54165509259259259</v>
+      </c>
+      <c r="N22" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O22" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P22" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R22" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24" t="s">
         <v>19</v>
       </c>
-      <c r="B21">
+      <c r="B24">
         <f>WEEKDAY(B1)</f>
         <v>7</v>
       </c>
-      <c r="C21">
-        <f t="shared" ref="C21:R21" si="2">WEEKDAY(C1)</f>
+      <c r="C24">
+        <f t="shared" ref="C24:R24" si="6">WEEKDAY(C1)</f>
         <v>7</v>
       </c>
-      <c r="D21">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="2"/>
+      <c r="D24">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="F21">
-        <f t="shared" si="2"/>
+      <c r="F24">
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="G21">
-        <f t="shared" si="2"/>
+      <c r="G24">
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="H21">
-        <f t="shared" si="2"/>
+      <c r="H24">
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="I21">
-        <f t="shared" si="2"/>
+      <c r="I24">
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="J21">
-        <f t="shared" si="2"/>
+      <c r="J24">
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="K21">
-        <f t="shared" si="2"/>
+      <c r="K24">
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="L21">
-        <f t="shared" si="2"/>
+      <c r="L24">
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="M21">
-        <f t="shared" si="2"/>
+      <c r="M24">
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="N21">
-        <f t="shared" si="2"/>
+      <c r="N24">
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="O21">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P21" t="e">
-        <f t="shared" si="2"/>
+      <c r="O24">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P24" t="e">
+        <f t="shared" si="6"/>
         <v>#NUM!</v>
       </c>
-      <c r="Q21" t="e">
-        <f t="shared" si="2"/>
+      <c r="Q24" t="e">
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R21" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18">
-      <c r="A24" t="s">
-        <v>22</v>
+      <c r="R24" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="25" spans="1:18">
       <c r="A25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="A28" t="s">
         <v>23</v>
       </c>
-      <c r="B25">
+      <c r="B28">
         <f>YEAR(B1)</f>
         <v>1900</v>
       </c>
-      <c r="C25">
-        <f t="shared" ref="C25:R25" si="3">YEAR(C1)</f>
+      <c r="C28">
+        <f t="shared" ref="C28:R28" si="7">YEAR(C1)</f>
         <v>1900</v>
       </c>
-      <c r="D25">
-        <f t="shared" si="3"/>
+      <c r="D28">
+        <f t="shared" si="7"/>
         <v>1900</v>
       </c>
-      <c r="E25">
-        <f t="shared" si="3"/>
+      <c r="E28">
+        <f t="shared" si="7"/>
         <v>1900</v>
       </c>
-      <c r="F25">
-        <f t="shared" si="3"/>
+      <c r="F28">
+        <f t="shared" si="7"/>
         <v>1900</v>
       </c>
-      <c r="G25">
-        <f t="shared" si="3"/>
+      <c r="G28">
+        <f t="shared" si="7"/>
         <v>1900</v>
       </c>
-      <c r="H25">
-        <f t="shared" si="3"/>
+      <c r="H28">
+        <f t="shared" si="7"/>
         <v>1900</v>
       </c>
-      <c r="I25">
-        <f t="shared" si="3"/>
+      <c r="I28">
+        <f t="shared" si="7"/>
         <v>1900</v>
       </c>
-      <c r="J25">
-        <f t="shared" si="3"/>
+      <c r="J28">
+        <f t="shared" si="7"/>
         <v>1900</v>
       </c>
-      <c r="K25">
-        <f t="shared" si="3"/>
+      <c r="K28">
+        <f t="shared" si="7"/>
         <v>1900</v>
       </c>
-      <c r="L25">
-        <f t="shared" si="3"/>
+      <c r="L28">
+        <f t="shared" si="7"/>
         <v>1901</v>
       </c>
-      <c r="M25">
-        <f t="shared" si="3"/>
+      <c r="M28">
+        <f t="shared" si="7"/>
         <v>1927</v>
       </c>
-      <c r="N25">
-        <f t="shared" si="3"/>
+      <c r="N28">
+        <f t="shared" si="7"/>
         <v>1900</v>
       </c>
-      <c r="O25">
-        <f t="shared" si="3"/>
+      <c r="O28">
+        <f t="shared" si="7"/>
         <v>1900</v>
       </c>
-      <c r="P25" t="e">
-        <f t="shared" si="3"/>
+      <c r="P28" t="e">
+        <f t="shared" si="7"/>
         <v>#NUM!</v>
       </c>
-      <c r="Q25" t="e">
-        <f t="shared" si="3"/>
+      <c r="Q28" t="e">
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R25" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18">
-      <c r="A26" t="s">
+      <c r="R28" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add edate() and eomonth() function
</commit_message>
<xml_diff>
--- a/tests/fixtures/date-time.xlsx
+++ b/tests/fixtures/date-time.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>date</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>12:59:59</t>
+  </si>
+  <si>
+    <t>50</t>
   </si>
 </sst>
 </file>
@@ -126,8 +129,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -165,8 +168,8 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -586,16 +589,50 @@
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="D3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3" s="1">
+        <f>100+C3</f>
+        <v>200</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:M3" si="0">100+D3</f>
+        <v>300</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
+        <f t="shared" si="0"/>
+        <v>101</v>
+      </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="3"/>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
       <c r="D4" s="1"/>
       <c r="I4" s="1"/>
       <c r="K4" s="1"/>
@@ -604,671 +641,817 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>0</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="3"/>
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <f>DAY(B1)</f>
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <f t="shared" ref="C8:R8" si="0">DAY(C1)</f>
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="P8" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="Q8" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R8" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <f>DAY(B1)</f>
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:R9" si="1">DAY(C1)</f>
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P9" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q9" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R9" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="10" spans="1:18">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <f>EDATE(B1+100,B3)</f>
+        <v>100</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:R12" si="2">EDATE(C1+100,C3)</f>
+        <v>3144</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>6189</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>9262</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>12308</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>15380</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>18423</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>21467</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>1683</v>
+      </c>
+      <c r="K12" t="e">
+        <f t="shared" ref="K12:Q12" si="3">EDATE(K1,K3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L12" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="3"/>
+        <v>13075</v>
+      </c>
+      <c r="N12" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O12" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P12" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q12" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R12" t="e">
+        <f>EDATE(R1,R3)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13">
-        <f>HOUR(B2)</f>
-        <v>0</v>
+        <f>EOMONTH(B1 + 100,B3)</f>
+        <v>121</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:R13" si="1">HOUR(C2)</f>
-        <v>14</v>
+        <f t="shared" ref="C13:R13" si="4">EOMONTH(C1 + 100,C3)</f>
+        <v>3166</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>6210</v>
       </c>
       <c r="E13">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>9283</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f t="shared" si="4"/>
+        <v>12327</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f t="shared" si="4"/>
+        <v>15400</v>
       </c>
       <c r="H13">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>18444</v>
       </c>
       <c r="I13">
-        <f t="shared" si="1"/>
-        <v>16</v>
+        <f t="shared" si="4"/>
+        <v>21489</v>
       </c>
       <c r="J13">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>1705</v>
+      </c>
+      <c r="K13" t="e">
+        <f t="shared" ref="K13:Q13" si="5">EOMONTH(K1,K3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L13" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
       </c>
       <c r="M13">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="N13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>13088</v>
+      </c>
+      <c r="N13" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O13" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
       </c>
       <c r="P13" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="Q13" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R13" t="e">
-        <f t="shared" si="1"/>
+        <f>EOMONTH(R1,R3)</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <f>HOUR(B2)</f>
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:R14" si="6">HOUR(C2)</f>
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P14" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q14" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R14" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="15" spans="1:18">
       <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15">
-        <f>MINUTE(B2)</f>
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <f t="shared" ref="C15:R15" si="2">MINUTE(C2)</f>
-        <v>24</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="2"/>
-        <v>45</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="2"/>
-        <v>59</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="2"/>
-        <v>59</v>
-      </c>
-      <c r="N15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P15" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="Q15" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R15" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <f>MINUTE(B2)</f>
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:R16" si="7">MINUTE(C2)</f>
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="7"/>
+        <v>23</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="7"/>
+        <v>23</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="7"/>
+        <v>45</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="7"/>
+        <v>23</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="7"/>
+        <v>59</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="7"/>
+        <v>59</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P16" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q16" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R16" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" t="s">
         <v>11</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <f>MONTH(B1)</f>
         <v>1</v>
       </c>
-      <c r="C16">
-        <f t="shared" ref="C16:O16" si="3">MONTH(C1)</f>
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="3"/>
+      <c r="C17">
+        <f t="shared" ref="C17:O17" si="8">MONTH(C1)</f>
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="G16">
-        <f t="shared" si="3"/>
+      <c r="G17">
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="H16">
-        <f t="shared" si="3"/>
+      <c r="H17">
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="I16">
-        <f t="shared" si="3"/>
+      <c r="I17">
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="J16">
-        <f t="shared" si="3"/>
+      <c r="J17">
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="K16">
-        <f t="shared" si="3"/>
+      <c r="K17">
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
-      <c r="L16">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="3"/>
+      <c r="L17">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="N16">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="P16" t="e">
+      <c r="N17">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="P17" t="e">
         <f>MONTH(P1)</f>
         <v>#NUM!</v>
       </c>
-      <c r="Q16" t="e">
+      <c r="Q17" t="e">
         <f>MONTH(Q1)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R16" t="e">
+      <c r="R17" t="e">
         <f>MONTH(R1)</f>
         <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18">
-      <c r="A17" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:18">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:18">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20">
-        <f>SECOND(B2)</f>
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <f t="shared" ref="C20:R20" si="4">SECOND(C2)</f>
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="4"/>
-        <v>36</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J20" s="7">
-        <f t="shared" si="4"/>
-        <v>54</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="4"/>
-        <v>59</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="4"/>
-        <v>59</v>
-      </c>
-      <c r="N20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P20" t="e">
-        <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="Q20" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R20" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:18">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <f>SECOND(B2)</f>
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21:R21" si="9">SECOND(C2)</f>
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="9"/>
+        <v>36</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="7">
+        <f t="shared" si="9"/>
+        <v>54</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="9"/>
+        <v>59</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="9"/>
+        <v>59</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P21" t="e">
+        <f t="shared" si="9"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q21" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R21" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="22" spans="1:18">
       <c r="A22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" t="e">
-        <f>TIMEVALUE(B2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C22" t="e">
-        <f t="shared" ref="C22:R22" si="5">TIMEVALUE(C2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D22" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="5"/>
-        <v>5.7638888888888885E-2</v>
-      </c>
-      <c r="F22" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G22" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H22" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I22" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J22" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="5"/>
-        <v>4.1655092592592598E-2</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="5"/>
-        <v>0.54165509259259259</v>
-      </c>
-      <c r="N22" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O22" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P22" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q22" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R22" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:18">
       <c r="A23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="B23" t="e">
+        <f>TIMEVALUE(B2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C23" t="e">
+        <f t="shared" ref="C23:R23" si="10">TIMEVALUE(C2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D23" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="10"/>
+        <v>5.7638888888888885E-2</v>
+      </c>
+      <c r="F23" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G23" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H23" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I23" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J23" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="10"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="10"/>
+        <v>4.1655092592592598E-2</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="10"/>
+        <v>0.54165509259259259</v>
+      </c>
+      <c r="N23" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O23" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P23" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q23" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R23" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="24" spans="1:18">
       <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="4"/>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25" t="s">
         <v>19</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <f>WEEKDAY(B1)</f>
         <v>7</v>
       </c>
-      <c r="C24">
-        <f t="shared" ref="C24:R24" si="6">WEEKDAY(C1)</f>
+      <c r="C25">
+        <f t="shared" ref="C25:R25" si="11">WEEKDAY(C1)</f>
         <v>7</v>
       </c>
-      <c r="D24">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="6"/>
+      <c r="D25">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
-      <c r="F24">
-        <f t="shared" si="6"/>
+      <c r="F25">
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="G24">
-        <f t="shared" si="6"/>
+      <c r="G25">
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="H24">
-        <f t="shared" si="6"/>
+      <c r="H25">
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
-      <c r="I24">
-        <f t="shared" si="6"/>
+      <c r="I25">
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
-      <c r="J24">
-        <f t="shared" si="6"/>
+      <c r="J25">
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
-      <c r="K24">
-        <f t="shared" si="6"/>
+      <c r="K25">
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
-      <c r="L24">
-        <f t="shared" si="6"/>
+      <c r="L25">
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
-      <c r="M24">
-        <f t="shared" si="6"/>
+      <c r="M25">
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="N24">
-        <f t="shared" si="6"/>
+      <c r="N25">
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
-      <c r="O24">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="P24" t="e">
-        <f t="shared" si="6"/>
+      <c r="O25">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="P25" t="e">
+        <f t="shared" si="11"/>
         <v>#NUM!</v>
       </c>
-      <c r="Q24" t="e">
-        <f t="shared" si="6"/>
+      <c r="Q25" t="e">
+        <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R24" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18">
-      <c r="A25" t="s">
-        <v>20</v>
+      <c r="R25" t="e">
+        <f t="shared" si="11"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="26" spans="1:18">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:18">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:18">
       <c r="A28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29" t="s">
         <v>23</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <f>YEAR(B1)</f>
         <v>1900</v>
       </c>
-      <c r="C28">
-        <f t="shared" ref="C28:R28" si="7">YEAR(C1)</f>
+      <c r="C29">
+        <f t="shared" ref="C29:R29" si="12">YEAR(C1)</f>
         <v>1900</v>
       </c>
-      <c r="D28">
-        <f t="shared" si="7"/>
+      <c r="D29">
+        <f t="shared" si="12"/>
         <v>1900</v>
       </c>
-      <c r="E28">
-        <f t="shared" si="7"/>
+      <c r="E29">
+        <f t="shared" si="12"/>
         <v>1900</v>
       </c>
-      <c r="F28">
-        <f t="shared" si="7"/>
+      <c r="F29">
+        <f t="shared" si="12"/>
         <v>1900</v>
       </c>
-      <c r="G28">
-        <f t="shared" si="7"/>
+      <c r="G29">
+        <f t="shared" si="12"/>
         <v>1900</v>
       </c>
-      <c r="H28">
-        <f t="shared" si="7"/>
+      <c r="H29">
+        <f t="shared" si="12"/>
         <v>1900</v>
       </c>
-      <c r="I28">
-        <f t="shared" si="7"/>
+      <c r="I29">
+        <f t="shared" si="12"/>
         <v>1900</v>
       </c>
-      <c r="J28">
-        <f t="shared" si="7"/>
+      <c r="J29">
+        <f t="shared" si="12"/>
         <v>1900</v>
       </c>
-      <c r="K28">
-        <f t="shared" si="7"/>
+      <c r="K29">
+        <f t="shared" si="12"/>
         <v>1900</v>
       </c>
-      <c r="L28">
-        <f t="shared" si="7"/>
+      <c r="L29">
+        <f t="shared" si="12"/>
         <v>1901</v>
       </c>
-      <c r="M28">
-        <f t="shared" si="7"/>
+      <c r="M29">
+        <f t="shared" si="12"/>
         <v>1927</v>
       </c>
-      <c r="N28">
-        <f t="shared" si="7"/>
+      <c r="N29">
+        <f t="shared" si="12"/>
         <v>1900</v>
       </c>
-      <c r="O28">
-        <f t="shared" si="7"/>
+      <c r="O29">
+        <f t="shared" si="12"/>
         <v>1900</v>
       </c>
-      <c r="P28" t="e">
-        <f t="shared" si="7"/>
+      <c r="P29" t="e">
+        <f t="shared" si="12"/>
         <v>#NUM!</v>
       </c>
-      <c r="Q28" t="e">
-        <f t="shared" si="7"/>
+      <c r="Q29" t="e">
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R28" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18">
-      <c r="A29" t="s">
+      <c r="R29" t="e">
+        <f t="shared" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="A30" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>